<commit_message>
Alteração para diferentes tipos de bimestrais
</commit_message>
<xml_diff>
--- a/data/teacher/Cleidson.xlsx
+++ b/data/teacher/Cleidson.xlsx
@@ -547,12 +547,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MCT-1A-Circuitos elétricos</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>MCT-1A-Maquinas eletricas</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -611,17 +611,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MCT-1A-Circuitos elétricos</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>MCT-1A-Maquinas eletricas</t>
+          <t>MCT-3A-Máquinas Elétricas</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MCT-1A-Circuitos elétricos</t>
         </is>
       </c>
     </row>
@@ -648,12 +648,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MCT-3A-Máquinas Elétricas</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MCT-1A-Circuitos elétricos</t>
         </is>
       </c>
     </row>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>['ELM-2NA-Automação Industrial', 'ELM-2NA-Automação Industrial', 'ELM-2NA-Automação Industrial', 'ELM-2NA-Automação Industrial']</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>['ELM-1NA-Sistemas Digitais', 'ELM-1NA-Sistemas Digitais', 'ELM-1NA-Sistemas Digitais', 'ELM-1NA-Sistemas Digitais']</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">

</xml_diff>